<commit_message>
Final changes on submission_file.xlsx
</commit_message>
<xml_diff>
--- a/submission_file.xlsx
+++ b/submission_file.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,29 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19034\Desktop\rice_datathon_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E7D1656D-1EBB-4368-B707-150A688BC743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B87B64-2B9B-4AED-8F41-AFA50BB85491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="submission_file" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>Predicted</t>
-  </si>
-  <si>
-    <t>Actual</t>
-  </si>
-  <si>
     <t>North Carolina</t>
   </si>
   <si>
@@ -79,9 +86,6 @@
     <t>Nevada</t>
   </si>
   <si>
-    <t>TEST RMSE:</t>
-  </si>
-  <si>
     <t>Idaho</t>
   </si>
   <si>
@@ -182,12 +186,15 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>TotalAmountofAssistance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,12 +509,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -671,10 +672,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1029,742 +1028,434 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G45" sqref="G45:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B2">
-        <v>145329171.90000001</v>
-      </c>
-      <c r="C2">
-        <v>176369306</v>
-      </c>
-      <c r="D2" s="1">
-        <v>19269800000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2295061.523</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>3855661.3769999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>38667417.969999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>27114375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>43555589.840000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>2617098.145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>7108524.4139999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>8170080.5659999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>35840179.689999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>26317662.109999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>8778904.2970000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>21791615.23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>8487153.3200000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>3977305.176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>80091250</v>
-      </c>
-      <c r="C3">
-        <v>145497267</v>
-      </c>
-      <c r="D3" s="1">
-        <v>85558900000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>56387894.530000001</v>
-      </c>
-      <c r="C4">
-        <v>5171076</v>
-      </c>
-      <c r="D4" s="1">
-        <v>52463300000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>43555589.840000004</v>
-      </c>
-      <c r="C5">
-        <v>58722209</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4600530000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>38667417.969999999</v>
-      </c>
-      <c r="C6">
-        <v>23756565</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4446670000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>35840179.689999998</v>
-      </c>
-      <c r="C7">
-        <v>8467648</v>
-      </c>
-      <c r="D7" s="1">
-        <v>14985100000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>28269441.41</v>
-      </c>
-      <c r="C8">
-        <v>2102663</v>
-      </c>
-      <c r="D8" s="1">
-        <v>13694000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>27760693.359999999</v>
-      </c>
-      <c r="C9">
-        <v>39346669</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2684700000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>27260720.699999999</v>
-      </c>
-      <c r="C10">
-        <v>39546994</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3019050000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>27114375</v>
-      </c>
-      <c r="C11">
-        <v>61208016</v>
-      </c>
-      <c r="D11" s="1">
-        <v>23247500000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>26317662.109999999</v>
-      </c>
-      <c r="C12">
-        <v>7307409</v>
-      </c>
-      <c r="D12" s="1">
-        <v>7227790000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>25095373.050000001</v>
-      </c>
-      <c r="C13">
-        <v>53672</v>
-      </c>
-      <c r="D13" s="1">
-        <v>12541700000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>21791615.23</v>
-      </c>
-      <c r="C14">
-        <v>733911</v>
-      </c>
-      <c r="D14" s="1">
-        <v>8868540000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>19603326.170000002</v>
-      </c>
-      <c r="C15">
-        <v>2509973</v>
-      </c>
-      <c r="D15" s="1">
-        <v>5843650000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
       <c r="B16">
-        <v>19289552.73</v>
-      </c>
-      <c r="C16">
-        <v>29357835</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2027410000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15098248.050000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>18471748.050000001</v>
-      </c>
-      <c r="C17">
-        <v>25808865</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1076670000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3634328.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>16474259.77</v>
       </c>
-      <c r="C18">
-        <v>11046095</v>
-      </c>
-      <c r="D18" s="1">
-        <v>589299000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>56387894.530000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>11624118.16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>7725035.6449999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>8034790.5269999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>5654900.8789999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>19289552.73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>28269441.41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B19">
-        <v>15488563.48</v>
-      </c>
-      <c r="C19">
-        <v>9860324</v>
-      </c>
-      <c r="D19" s="1">
-        <v>633542000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>15098248.050000001</v>
-      </c>
-      <c r="C20">
-        <v>63476066</v>
-      </c>
-      <c r="D20" s="1">
-        <v>46808300000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21">
-        <v>13441389.65</v>
-      </c>
-      <c r="C21">
-        <v>6976448</v>
-      </c>
-      <c r="D21" s="1">
-        <v>835909000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22">
-        <v>11624118.16</v>
-      </c>
-      <c r="C22">
-        <v>1718854</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1962290000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23">
+      <c r="B26">
         <v>11447896.48</v>
       </c>
-      <c r="C23">
-        <v>4677028</v>
-      </c>
-      <c r="D23" s="1">
-        <v>916893000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24">
-        <v>10763815.43</v>
-      </c>
-      <c r="C24">
-        <v>2405926</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1397090000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>4806627.4409999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>28</v>
-      </c>
-      <c r="B25">
-        <v>9468893.5549999997</v>
-      </c>
-      <c r="C25">
-        <v>2039514</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1103910000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26">
-        <v>9117534.1799999997</v>
-      </c>
-      <c r="C26">
-        <v>996776</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1318930000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27">
-        <v>8778904.2970000003</v>
-      </c>
-      <c r="C27">
-        <v>1153848</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1162830000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="B28">
         <v>8625490.2339999992</v>
       </c>
-      <c r="C28">
-        <v>9134015</v>
-      </c>
-      <c r="D28">
-        <v>5171948745</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>25095373.050000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>9117534.1799999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>6437005.8590000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>1992676.514</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>27760693.359999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>145329171.90000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35">
+        <v>2240082.52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>7426227.051</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37">
+        <v>3792859.8629999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>18471748.050000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>6048299.3159999996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
-        <v>8487153.3200000003</v>
-      </c>
-      <c r="C29">
-        <v>3526853</v>
-      </c>
-      <c r="D29" s="1">
-        <v>492092000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30">
-        <v>8170080.5659999996</v>
-      </c>
-      <c r="C30">
-        <v>23750266</v>
-      </c>
-      <c r="D30" s="1">
-        <v>4854840000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B40">
+        <v>7833557.6169999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>80091250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42">
+        <v>13441389.65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
-      <c r="B31">
-        <v>8034790.5269999998</v>
-      </c>
-      <c r="C31">
-        <v>21021782</v>
-      </c>
-      <c r="D31" s="1">
-        <v>3373240000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32">
-        <v>7833557.6169999996</v>
-      </c>
-      <c r="C32">
-        <v>635939</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1036110000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33">
-        <v>7725035.6449999996</v>
-      </c>
-      <c r="C33">
-        <v>1459180</v>
-      </c>
-      <c r="D33" s="1">
-        <v>785219000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34">
+      <c r="B43">
         <v>7514987.7929999996</v>
       </c>
-      <c r="C34">
-        <v>1536871</v>
-      </c>
-      <c r="D34" s="1">
-        <v>714758000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35">
-        <v>7426227.051</v>
-      </c>
-      <c r="C35">
-        <v>3038155</v>
-      </c>
-      <c r="D35" s="1">
-        <v>385104000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36">
-        <v>7108524.4139999999</v>
-      </c>
-      <c r="C36">
-        <v>491729</v>
-      </c>
-      <c r="D36" s="1">
-        <v>875640000000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37">
-        <v>6437005.8590000002</v>
-      </c>
-      <c r="C37">
-        <v>428543</v>
-      </c>
-      <c r="D37" s="1">
-        <v>722033000000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38">
-        <v>6048299.3159999996</v>
-      </c>
-      <c r="C38">
-        <v>2136747</v>
-      </c>
-      <c r="D38" s="1">
-        <v>306005000000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39">
-        <v>5654900.8789999997</v>
-      </c>
-      <c r="C39">
-        <v>3543100</v>
-      </c>
-      <c r="D39">
-        <v>89194059043</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40">
-        <v>4806627.4409999996</v>
-      </c>
-      <c r="C40">
-        <v>542585</v>
-      </c>
-      <c r="D40" s="1">
-        <v>363641000000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41">
-        <v>3977305.176</v>
-      </c>
-      <c r="C41">
-        <v>8555854</v>
-      </c>
-      <c r="D41" s="1">
-        <v>419262000000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42">
-        <v>3855661.3769999999</v>
-      </c>
-      <c r="C42">
-        <v>9567164</v>
-      </c>
-      <c r="D42" s="1">
-        <v>652425000000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43">
-        <v>3792859.8629999999</v>
-      </c>
-      <c r="C43">
-        <v>560909</v>
-      </c>
-      <c r="D43" s="1">
-        <v>208910000000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B44">
-        <v>3634328.125</v>
-      </c>
-      <c r="C44">
-        <v>2802130</v>
-      </c>
-      <c r="D44">
-        <v>13851074385</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+        <v>27260720.699999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>48</v>
       </c>
       <c r="B45">
-        <v>2617098.145</v>
-      </c>
-      <c r="C45">
-        <v>6304206</v>
-      </c>
-      <c r="D45" s="1">
-        <v>271895000000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1787613.037</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>10763815.43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>9468893.5549999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>19603326.170000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B46">
-        <v>2295061.523</v>
-      </c>
-      <c r="C46">
-        <v>1174323</v>
-      </c>
-      <c r="D46">
-        <v>25121096758</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="B49">
+        <v>1707258.301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>15488563.48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>50</v>
-      </c>
-      <c r="B47">
-        <v>2240082.52</v>
-      </c>
-      <c r="C47">
-        <v>686913</v>
-      </c>
-      <c r="D47">
-        <v>48246711128</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48">
-        <v>1992676.514</v>
-      </c>
-      <c r="C48">
-        <v>48503359</v>
-      </c>
-      <c r="D48" s="1">
-        <v>43264900000000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49">
-        <v>1787613.037</v>
-      </c>
-      <c r="C49">
-        <v>736194</v>
-      </c>
-      <c r="D49">
-        <v>22109639832</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50">
-        <v>1707258.301</v>
-      </c>
-      <c r="C50">
-        <v>1052654</v>
-      </c>
-      <c r="D50">
-        <v>8570135812</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>53</v>
       </c>
       <c r="B51">
         <v>-293223.84639999998</v>
       </c>
-      <c r="C51">
-        <v>229763</v>
-      </c>
-      <c r="D51">
-        <v>5470304831</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C52" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="2">
-        <v>19422361.23</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B52">
+    <sortCondition ref="A1:A52"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>